<commit_message>
updated version info in templates
</commit_message>
<xml_diff>
--- a/oci_tenancy/SetUpOCI_Via_TF/example/CD3-DRGv2-template.xlsx
+++ b/oci_tenancy/SetUpOCI_Via_TF/example/CD3-DRGv2-template.xlsx
@@ -6606,77 +6606,6 @@
                                 Example: Operations.CostCenter=01;Users.Name=user01</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Automation Toolkit</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>release version-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">v8.0
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Added new sheets - DRGs and DRGRouteRulesinOCI
-</t>
-    </r>
-  </si>
-  <si>
     <t xml:space="preserve"># Rows after &lt;END&gt; will not be processed (Sample data is provided for reference after &lt;END&gt;).
 - Columns Region, Compartment Name, DRG Name are mandatory.
 - Leave columns DRG RT Name,  Import DRG Route Distribution Name and Import DRG   Route Distribution Statements empty to use Autogenerated ones.
@@ -6868,6 +6797,77 @@
   </si>
   <si>
     <t>10.110.3.0/24</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Automation Toolkit</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>release version-</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">v8.0.2
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Added new sheets - DRGs and DRGRouteRulesinOCI
+</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -9586,7 +9586,7 @@
     <row r="1" spans="1:1" ht="15" thickBot="1"/>
     <row r="2" spans="1:1" ht="59" customHeight="1" thickBot="1">
       <c r="A2" s="80" t="s">
-        <v>884</v>
+        <v>943</v>
       </c>
     </row>
   </sheetData>
@@ -9712,10 +9712,10 @@
         <v>376</v>
       </c>
       <c r="C3" s="41" t="s">
-        <v>920</v>
+        <v>919</v>
       </c>
       <c r="D3" s="41" t="s">
-        <v>928</v>
+        <v>927</v>
       </c>
       <c r="E3" s="41" t="s">
         <v>51</v>
@@ -9730,10 +9730,10 @@
         <v>36</v>
       </c>
       <c r="I3" s="41" t="s">
-        <v>931</v>
+        <v>930</v>
       </c>
       <c r="J3" s="39" t="s">
-        <v>934</v>
+        <v>933</v>
       </c>
       <c r="K3" s="36" t="s">
         <v>23</v>
@@ -9764,10 +9764,10 @@
         <v>376</v>
       </c>
       <c r="C4" s="41" t="s">
-        <v>920</v>
+        <v>919</v>
       </c>
       <c r="D4" s="41" t="s">
-        <v>929</v>
+        <v>928</v>
       </c>
       <c r="E4" s="41" t="s">
         <v>798</v>
@@ -9782,10 +9782,10 @@
         <v>36</v>
       </c>
       <c r="I4" s="41" t="s">
-        <v>932</v>
+        <v>931</v>
       </c>
       <c r="J4" s="39" t="s">
-        <v>935</v>
+        <v>934</v>
       </c>
       <c r="K4" s="36" t="s">
         <v>23</v>
@@ -9816,13 +9816,13 @@
         <v>376</v>
       </c>
       <c r="C5" s="41" t="s">
-        <v>920</v>
+        <v>919</v>
       </c>
       <c r="D5" s="41" t="s">
-        <v>930</v>
+        <v>929</v>
       </c>
       <c r="E5" s="41" t="s">
-        <v>943</v>
+        <v>942</v>
       </c>
       <c r="F5" s="41" t="s">
         <v>52</v>
@@ -9834,10 +9834,10 @@
         <v>36</v>
       </c>
       <c r="I5" s="41" t="s">
-        <v>933</v>
+        <v>932</v>
       </c>
       <c r="J5" s="39" t="s">
-        <v>936</v>
+        <v>935</v>
       </c>
       <c r="K5" s="41" t="s">
         <v>23</v>
@@ -10635,20 +10635,20 @@
         <v>795</v>
       </c>
       <c r="D3" s="39" t="s">
-        <v>925</v>
+        <v>924</v>
       </c>
       <c r="E3" s="39"/>
       <c r="F3" s="75" t="s">
         <v>29</v>
       </c>
       <c r="G3" s="75" t="s">
-        <v>937</v>
+        <v>936</v>
       </c>
       <c r="H3" s="75" t="s">
         <v>829</v>
       </c>
       <c r="I3" s="39" t="s">
-        <v>939</v>
+        <v>938</v>
       </c>
       <c r="J3" s="39"/>
       <c r="K3" s="41"/>
@@ -14292,13 +14292,13 @@
         <v>140</v>
       </c>
       <c r="D2" s="21" t="s">
+        <v>939</v>
+      </c>
+      <c r="E2" s="21" t="s">
         <v>940</v>
       </c>
-      <c r="E2" s="21" t="s">
+      <c r="F2" s="21" t="s">
         <v>941</v>
-      </c>
-      <c r="F2" s="21" t="s">
-        <v>942</v>
       </c>
       <c r="G2" s="21" t="s">
         <v>141</v>
@@ -18438,10 +18438,10 @@
         <v>5</v>
       </c>
       <c r="B10" s="39" t="s">
+        <v>886</v>
+      </c>
+      <c r="C10" s="39" t="s">
         <v>887</v>
-      </c>
-      <c r="C10" s="39" t="s">
-        <v>888</v>
       </c>
       <c r="D10" s="39"/>
       <c r="E10" s="39"/>
@@ -18544,7 +18544,7 @@
       <c r="C4" s="39"/>
       <c r="D4" s="39"/>
       <c r="E4" s="39" t="s">
-        <v>889</v>
+        <v>888</v>
       </c>
       <c r="F4" s="39"/>
       <c r="G4" s="39"/>
@@ -18828,7 +18828,7 @@
       <c r="C27" s="39"/>
       <c r="D27" s="39"/>
       <c r="E27" s="39" t="s">
-        <v>890</v>
+        <v>889</v>
       </c>
       <c r="F27" s="39"/>
       <c r="G27" s="39"/>
@@ -18852,7 +18852,7 @@
       <c r="C29" s="39"/>
       <c r="D29" s="39"/>
       <c r="E29" s="39" t="s">
-        <v>891</v>
+        <v>890</v>
       </c>
       <c r="F29" s="39"/>
       <c r="G29" s="39"/>
@@ -18864,7 +18864,7 @@
       <c r="C30" s="39"/>
       <c r="D30" s="39"/>
       <c r="E30" s="39" t="s">
-        <v>892</v>
+        <v>891</v>
       </c>
       <c r="F30" s="39"/>
       <c r="G30" s="39"/>
@@ -18924,7 +18924,7 @@
       <c r="C35" s="39"/>
       <c r="D35" s="39"/>
       <c r="E35" s="39" t="s">
-        <v>893</v>
+        <v>892</v>
       </c>
       <c r="F35" s="39"/>
       <c r="G35" s="39"/>
@@ -18936,7 +18936,7 @@
       <c r="C36" s="39"/>
       <c r="D36" s="39"/>
       <c r="E36" s="39" t="s">
-        <v>894</v>
+        <v>893</v>
       </c>
       <c r="F36" s="39"/>
       <c r="G36" s="39"/>
@@ -19100,7 +19100,7 @@
       <c r="C49" s="39"/>
       <c r="D49" s="39"/>
       <c r="E49" s="39" t="s">
-        <v>895</v>
+        <v>894</v>
       </c>
       <c r="F49" s="39"/>
       <c r="G49" s="39"/>
@@ -19112,7 +19112,7 @@
       <c r="C50" s="39"/>
       <c r="D50" s="39"/>
       <c r="E50" s="39" t="s">
-        <v>896</v>
+        <v>895</v>
       </c>
       <c r="F50" s="39"/>
       <c r="G50" s="39"/>
@@ -19123,16 +19123,16 @@
         <v>5</v>
       </c>
       <c r="B51" s="39" t="s">
-        <v>897</v>
+        <v>896</v>
       </c>
       <c r="C51" s="39" t="s">
         <v>428</v>
       </c>
       <c r="D51" s="39" t="s">
+        <v>897</v>
+      </c>
+      <c r="E51" s="39" t="s">
         <v>898</v>
-      </c>
-      <c r="E51" s="39" t="s">
-        <v>899</v>
       </c>
       <c r="F51" s="39"/>
       <c r="G51" s="39"/>
@@ -19144,7 +19144,7 @@
       <c r="C52" s="39"/>
       <c r="D52" s="39"/>
       <c r="E52" s="39" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
       <c r="F52" s="39"/>
       <c r="G52" s="39"/>
@@ -19156,7 +19156,7 @@
       <c r="C53" s="39"/>
       <c r="D53" s="39"/>
       <c r="E53" s="39" t="s">
-        <v>901</v>
+        <v>900</v>
       </c>
       <c r="F53" s="39"/>
       <c r="G53" s="39"/>
@@ -19168,7 +19168,7 @@
       <c r="C54" s="39"/>
       <c r="D54" s="39"/>
       <c r="E54" s="39" t="s">
-        <v>902</v>
+        <v>901</v>
       </c>
       <c r="F54" s="39"/>
       <c r="G54" s="39"/>
@@ -19604,7 +19604,7 @@
       <c r="C89" s="39"/>
       <c r="D89" s="39"/>
       <c r="E89" s="39" t="s">
-        <v>903</v>
+        <v>902</v>
       </c>
       <c r="F89" s="39"/>
       <c r="G89" s="39"/>
@@ -19616,7 +19616,7 @@
       <c r="C90" s="39"/>
       <c r="D90" s="39"/>
       <c r="E90" s="39" t="s">
-        <v>904</v>
+        <v>903</v>
       </c>
       <c r="F90" s="39"/>
       <c r="G90" s="39"/>
@@ -19636,7 +19636,7 @@
         <v>742</v>
       </c>
       <c r="E91" s="39" t="s">
-        <v>905</v>
+        <v>904</v>
       </c>
       <c r="F91" s="39"/>
       <c r="G91" s="39"/>
@@ -19720,7 +19720,7 @@
       <c r="C98" s="39"/>
       <c r="D98" s="39"/>
       <c r="E98" s="39" t="s">
-        <v>906</v>
+        <v>905</v>
       </c>
       <c r="F98" s="39"/>
       <c r="G98" s="39"/>
@@ -19744,7 +19744,7 @@
       <c r="C100" s="39"/>
       <c r="D100" s="39"/>
       <c r="E100" s="39" t="s">
-        <v>907</v>
+        <v>906</v>
       </c>
       <c r="F100" s="39"/>
       <c r="G100" s="39"/>
@@ -19756,7 +19756,7 @@
       <c r="C101" s="39"/>
       <c r="D101" s="39"/>
       <c r="E101" s="39" t="s">
-        <v>908</v>
+        <v>907</v>
       </c>
       <c r="F101" s="39"/>
       <c r="G101" s="39"/>
@@ -19768,7 +19768,7 @@
       <c r="C102" s="39"/>
       <c r="D102" s="39"/>
       <c r="E102" s="39" t="s">
-        <v>909</v>
+        <v>908</v>
       </c>
       <c r="F102" s="39"/>
       <c r="G102" s="39"/>
@@ -19816,7 +19816,7 @@
       <c r="C106" s="39"/>
       <c r="D106" s="39"/>
       <c r="E106" s="39" t="s">
-        <v>910</v>
+        <v>909</v>
       </c>
       <c r="F106" s="39"/>
       <c r="G106" s="39"/>
@@ -19828,7 +19828,7 @@
       <c r="C107" s="39"/>
       <c r="D107" s="39"/>
       <c r="E107" s="39" t="s">
-        <v>911</v>
+        <v>910</v>
       </c>
       <c r="F107" s="39"/>
       <c r="G107" s="39"/>
@@ -19840,7 +19840,7 @@
       <c r="C108" s="39"/>
       <c r="D108" s="39"/>
       <c r="E108" s="39" t="s">
-        <v>912</v>
+        <v>911</v>
       </c>
       <c r="F108" s="39"/>
       <c r="G108" s="39"/>
@@ -19980,7 +19980,7 @@
       <c r="C119" s="39"/>
       <c r="D119" s="39"/>
       <c r="E119" s="39" t="s">
-        <v>913</v>
+        <v>912</v>
       </c>
       <c r="F119" s="39"/>
       <c r="G119" s="39"/>
@@ -19992,7 +19992,7 @@
       <c r="C120" s="39"/>
       <c r="D120" s="39"/>
       <c r="E120" s="39" t="s">
-        <v>914</v>
+        <v>913</v>
       </c>
       <c r="F120" s="39"/>
       <c r="G120" s="39"/>
@@ -20056,7 +20056,7 @@
       <c r="C124" s="39"/>
       <c r="D124" s="39"/>
       <c r="E124" s="39" t="s">
-        <v>915</v>
+        <v>914</v>
       </c>
       <c r="F124" s="39"/>
       <c r="G124" s="39"/>
@@ -20344,7 +20344,7 @@
       <c r="C148" s="39"/>
       <c r="D148" s="39"/>
       <c r="E148" s="39" t="s">
-        <v>916</v>
+        <v>915</v>
       </c>
       <c r="F148" s="39"/>
       <c r="G148" s="39"/>
@@ -20356,7 +20356,7 @@
       <c r="C149" s="39"/>
       <c r="D149" s="39"/>
       <c r="E149" s="39" t="s">
-        <v>917</v>
+        <v>916</v>
       </c>
       <c r="F149" s="39"/>
       <c r="G149" s="39"/>
@@ -20404,7 +20404,7 @@
       <c r="C153" s="39"/>
       <c r="D153" s="39"/>
       <c r="E153" s="39" t="s">
-        <v>918</v>
+        <v>917</v>
       </c>
       <c r="F153" s="39"/>
       <c r="G153" s="39"/>
@@ -20893,7 +20893,7 @@
         <v>376</v>
       </c>
       <c r="C3" s="41" t="s">
-        <v>920</v>
+        <v>919</v>
       </c>
       <c r="D3" s="41" t="s">
         <v>20</v>
@@ -20914,7 +20914,7 @@
         <v>23</v>
       </c>
       <c r="J3" s="41" t="s">
-        <v>919</v>
+        <v>918</v>
       </c>
       <c r="K3" s="41"/>
       <c r="L3" s="39"/>
@@ -20948,7 +20948,7 @@
         <v>23</v>
       </c>
       <c r="J4" s="41" t="s">
-        <v>919</v>
+        <v>918</v>
       </c>
       <c r="K4" s="41"/>
       <c r="L4" s="35"/>
@@ -20982,7 +20982,7 @@
         <v>23</v>
       </c>
       <c r="J5" s="41" t="s">
-        <v>919</v>
+        <v>918</v>
       </c>
       <c r="K5" s="41"/>
       <c r="L5" s="35"/>
@@ -21079,14 +21079,14 @@
   <sheetData>
     <row r="1" spans="1:7" ht="222" customHeight="1">
       <c r="A1" s="95" t="s">
-        <v>885</v>
+        <v>884</v>
       </c>
       <c r="B1" s="96"/>
       <c r="C1" s="96"/>
       <c r="D1" s="96"/>
       <c r="E1" s="96"/>
       <c r="F1" s="95" t="s">
-        <v>886</v>
+        <v>885</v>
       </c>
       <c r="G1" s="96"/>
     </row>
@@ -21124,16 +21124,16 @@
         <v>795</v>
       </c>
       <c r="D3" s="39" t="s">
-        <v>921</v>
+        <v>920</v>
       </c>
       <c r="E3" s="39" t="s">
-        <v>924</v>
+        <v>923</v>
       </c>
       <c r="F3" s="39" t="s">
-        <v>926</v>
+        <v>925</v>
       </c>
       <c r="G3" s="39" t="s">
-        <v>938</v>
+        <v>937</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="29">
@@ -21147,10 +21147,10 @@
         <v>795</v>
       </c>
       <c r="D4" s="39" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="E4" s="39" t="s">
-        <v>925</v>
+        <v>924</v>
       </c>
       <c r="F4" s="39"/>
       <c r="G4" s="39"/>
@@ -21166,10 +21166,10 @@
         <v>795</v>
       </c>
       <c r="D5" s="39" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="E5" s="39" t="s">
-        <v>925</v>
+        <v>924</v>
       </c>
       <c r="F5" s="39"/>
       <c r="G5" s="39"/>
@@ -21562,7 +21562,7 @@
         <v>376</v>
       </c>
       <c r="C3" s="41" t="s">
-        <v>920</v>
+        <v>919</v>
       </c>
       <c r="D3" s="41" t="s">
         <v>36</v>
@@ -21571,7 +21571,7 @@
         <v>39</v>
       </c>
       <c r="F3" s="41" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
       <c r="G3" s="41"/>
       <c r="H3" s="41"/>
@@ -21593,7 +21593,7 @@
         <v>39</v>
       </c>
       <c r="F4" s="41" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
       <c r="G4" s="41"/>
       <c r="H4" s="41"/>
@@ -21615,7 +21615,7 @@
         <v>39</v>
       </c>
       <c r="F5" s="41" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
       <c r="G5" s="41"/>
       <c r="H5" s="41"/>

</xml_diff>